<commit_message>
Basic excel import and export working with tests as plugins.
</commit_message>
<xml_diff>
--- a/excel_api/RawData.xlsx
+++ b/excel_api/RawData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="519" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Data and Analysis" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="DataAnalysis" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -193,9 +193,9 @@
   <dimension ref="1:73"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="I81" activeCellId="0" sqref="I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>